<commit_message>
Working on mle optimization
</commit_message>
<xml_diff>
--- a/demo_files/mle/twitch/progress/best.xlsx
+++ b/demo_files/mle/twitch/progress/best.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,467 +480,129 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6187575873347572</v>
+        <v>0.5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6383068831217756</v>
+        <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5294509848962967</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.48755049694252</v>
+        <v>0.5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3997503729503316</v>
+        <v>0.5</v>
       </c>
       <c r="G2" t="n">
-        <v>185701041052.5473</v>
+        <v>159225120419.1541</v>
       </c>
       <c r="H2" t="n">
-        <v>185701041052.5473</v>
+        <v>159225120419.1541</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5182804472767302</v>
+        <v>0.6763105250948414</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2815030437247478</v>
+        <v>0.5639598069268966</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6364915716896611</v>
+        <v>0.4590975363117272</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4956011333261604</v>
+        <v>0.5784916603168814</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5349899609811598</v>
+        <v>0.6070562892020971</v>
       </c>
       <c r="G3" t="n">
-        <v>71373664935.91931</v>
+        <v>35256133824.5209</v>
       </c>
       <c r="H3" t="n">
-        <v>71373664935.91931</v>
+        <v>35256133824.5209</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5130859296159987</v>
+        <v>0.7018904719410097</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2840809777833732</v>
+        <v>0.5590093055963493</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6405352974357821</v>
+        <v>0.4721469277564656</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4706652328167416</v>
+        <v>0.6005476568857232</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5010798597138391</v>
+        <v>0.616793624332957</v>
       </c>
       <c r="G4" t="n">
-        <v>57334656092.82462</v>
+        <v>17568017822.7105</v>
       </c>
       <c r="H4" t="n">
-        <v>57334656092.82462</v>
+        <v>17568017822.7105</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>30</v>
+        <v>144</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4751613255425842</v>
+        <v>0.6166629667347234</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3117911722411841</v>
+        <v>0.5978053607225976</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3877482273752728</v>
+        <v>0.6362423275816746</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5635713739061234</v>
+        <v>0.7000084535165928</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6010339132285799</v>
+        <v>0.6291360141694249</v>
       </c>
       <c r="G5" t="n">
-        <v>46032889489.3438</v>
+        <v>14493734465.3352</v>
       </c>
       <c r="H5" t="n">
-        <v>46032889489.3438</v>
+        <v>14493734465.3352</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>58</v>
+        <v>175</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5397576601864773</v>
+        <v>0.5330344036114565</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3994937251593241</v>
+        <v>0.6411446259488361</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4072513952185425</v>
+        <v>0.5696293185298874</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5780436833071446</v>
+        <v>0.8876283346835775</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5814481006855305</v>
+        <v>0.7656143053069452</v>
       </c>
       <c r="G6" t="n">
-        <v>41343576810.8365</v>
+        <v>12561295098.8403</v>
       </c>
       <c r="H6" t="n">
-        <v>41343576810.8365</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>151</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.650311929954543</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.7850644406128806</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.3033052224415979</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.7695428079451158</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.6465431946912154</v>
-      </c>
-      <c r="G7" t="n">
-        <v>17594199683.76</v>
-      </c>
-      <c r="H7" t="n">
-        <v>17594199683.76</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>230</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.515495802479949</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.7659731216797379</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-0.371562867651938</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.9191439775191927</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.7732952443958422</v>
-      </c>
-      <c r="G8" t="n">
-        <v>15789825987.8382</v>
-      </c>
-      <c r="H8" t="n">
-        <v>15789825987.8382</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>345</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.511930058509139</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.5420105726738041</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.2529105856236876</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.7920242603721191</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.7132370499382188</v>
-      </c>
-      <c r="G9" t="n">
-        <v>11947132374.9261</v>
-      </c>
-      <c r="H9" t="n">
-        <v>11947132374.9261</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>498</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.5242982885443084</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.5569430619056879</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.2398626186496541</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.7856582187505887</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.7077265385217238</v>
-      </c>
-      <c r="G10" t="n">
-        <v>11907803235.4095</v>
-      </c>
-      <c r="H10" t="n">
-        <v>11907803235.4095</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>504</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.4086319065281142</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.3115194839904095</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.1641603505654048</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.8429792903115607</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.8319488867154846</v>
-      </c>
-      <c r="G11" t="n">
-        <v>11289074879.0372</v>
-      </c>
-      <c r="H11" t="n">
-        <v>11289074879.0372</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>605</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.3546592179317587</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.2365091610442975</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.1184267809041017</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.9619715281790597</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.9715846578468643</v>
-      </c>
-      <c r="G12" t="n">
-        <v>10606780757.6189</v>
-      </c>
-      <c r="H12" t="n">
-        <v>10606780757.6189</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>622</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0.7399398418972311</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.813590728505347</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-0.008176605789585768</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.6898627953211557</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.6295855643195079</v>
-      </c>
-      <c r="G13" t="n">
-        <v>9626023036.898201</v>
-      </c>
-      <c r="H13" t="n">
-        <v>9626023036.898201</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>744</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0.4967894672163221</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.5507781908345933</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.02521231520281095</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.9040364157485963</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.816796268394645</v>
-      </c>
-      <c r="G14" t="n">
-        <v>9619070583.232401</v>
-      </c>
-      <c r="H14" t="n">
-        <v>9619070583.232401</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>763</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.4072203207697956</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.3638876516225262</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.141113147323593</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.9498662675134668</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.904466672333968</v>
-      </c>
-      <c r="G15" t="n">
-        <v>5138311536.2348</v>
-      </c>
-      <c r="H15" t="n">
-        <v>5138311536.2348</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>2049</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0.7292943381894168</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.7639506567154531</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.06458180180508209</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.7626727562145892</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.696626660349279</v>
-      </c>
-      <c r="G16" t="n">
-        <v>4765132410.3905</v>
-      </c>
-      <c r="H16" t="n">
-        <v>4765132410.3905</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>2057</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.6751224598869265</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.6887380761755477</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.1199384407516041</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.8208547616514401</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.7532630232530811</v>
-      </c>
-      <c r="G17" t="n">
-        <v>4138107905.2437</v>
-      </c>
-      <c r="H17" t="n">
-        <v>4138107905.2437</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>2906</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.6748293073534875</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.7125037251467728</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.1282075643193015</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.7826595014585347</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.7103235229200121</v>
-      </c>
-      <c r="G18" t="n">
-        <v>4121057372.077099</v>
-      </c>
-      <c r="H18" t="n">
-        <v>4121057372.077099</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>3698</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.6703298052281137</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.7284935820480957</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.1761906146420112</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.7840790008484072</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.6983409116546613</v>
-      </c>
-      <c r="G19" t="n">
-        <v>3888763109.2823</v>
-      </c>
-      <c r="H19" t="n">
-        <v>3888763109.2823</v>
+        <v>12561295098.8403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>